<commit_message>
Added header data bag
</commit_message>
<xml_diff>
--- a/documents/Published/Dynamic Tooltip/DynamicTooltipByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Dynamic Tooltip/DynamicTooltipByMAQSoftwareChecklist.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Power BI\DynamicTooltip\5-9-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLab_PowerBIVisuals\documents\Published\Dynamic Tooltip\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E83897F-12A6-4E0F-8448-1E68803D41FA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="4935" activeTab="1" xr2:uid="{97DCB166-1937-475F-B7FA-86832FE14153}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="4935" xr2:uid="{97DCB166-1937-475F-B7FA-86832FE14153}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>S no</t>
   </si>
@@ -42,9 +43,6 @@
     <t>Basic dynamic tooltip</t>
   </si>
   <si>
-    <t>Drag 'Sales' in 'Values' field</t>
-  </si>
-  <si>
     <t>Measure Tooltip</t>
   </si>
   <si>
@@ -58,14 +56,6 @@
   </si>
   <si>
     <t>Dynamic tooltip with information will be displayed</t>
-  </si>
-  <si>
-    <t>1. Go to formatting pane
-2. Go to 'Tooltip' option
-3. Update 'Header' to 'The Title'
-4. Update 'Body' to 'This is body'
-5. Update 'Image URL' to 'https://d30y9cdsu7xlg0.cloudfront.net/png/205323-200.png'
-6. Switch 'Measure Tooltip' toggle OFF</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -163,23 +153,84 @@
     <t>Does visual legends adjusted on resizing? </t>
   </si>
   <si>
+    <t>Display basic dynamic tooltip</t>
+  </si>
+  <si>
+    <t>Does visual work properly on changing format in Modelling ribbon? Should match with other visuals behavior </t>
+  </si>
+  <si>
+    <t>Have we handled Zero and NULL values for axis/data values and labels properly? Should match with other visuals behavior.  </t>
+  </si>
+  <si>
+    <t>Expected output</t>
+  </si>
+  <si>
+    <t>Dynamic tooltip with information will be displayed with currency formatting like '$120'</t>
+  </si>
+  <si>
+    <t>Display basic dynamic tooltip with currency formatting</t>
+  </si>
+  <si>
+    <t>Display basic dynamic tooltip with numeric values</t>
+  </si>
+  <si>
+    <t>Display basic dynamic tooltip with Categorical values</t>
+  </si>
+  <si>
+    <t>1. Drag 'Order Quantity' Field in 'Body' field
+2. Hover on the visual</t>
+  </si>
+  <si>
+    <t>1. Drag 'Month' Field in 'Body'
+2. Hover on the visual</t>
+  </si>
+  <si>
+    <t>1. Drag 'Sales' Field in 'Header' field
+2. Drag 'Sales' in 'Body'  field 
+3. Hover on the visual</t>
+  </si>
+  <si>
+    <t>Same value shoud be displayed as header and Body</t>
+  </si>
+  <si>
+    <t>1. Drag 'Sales Header' Field in 'Header' field
+2. Drag 'Sales' in 'Body'  field 
+3. Hover on the visual</t>
+  </si>
+  <si>
+    <t>1. Dynamic tooltip with only Header Value will be displayed
+2. Dynamic tooltip with Header and Body will be displayed</t>
+  </si>
+  <si>
     <t>1. Go to formatting pane
-2. Go to 'Measure Tooltip' option
-3. Switch the toggle on
-4. Update 'decimal places' to '2'
-5. Update 'display units' to 'Thousand'</t>
-  </si>
-  <si>
-    <t>Display basic dynamic tooltip</t>
-  </si>
-  <si>
-    <t>Does visual work properly on changing format in Modelling ribbon? Should match with other visuals behavior </t>
-  </si>
-  <si>
-    <t>Have we handled Zero and NULL values for axis/data values and labels properly? Should match with other visuals behavior.  </t>
-  </si>
-  <si>
-    <t>Expected output</t>
+2. Switch the toggle of 'Measure Tooltip' option to ON
+3. Drag 'Sales' in 'Body'  field 
+4.Hover on the visual</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Switch the toggle of 'Measure Tooltip' option to ON
+3. Update 'decimal places' to '2'
+4. Update 'display units' to 'Thousand'</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Switch the toggle of 'Measure Tooltip' option to OFF
+3. Go to 'Tooltip' option
+4. Update 'Header' to 'The Title'
+5. Update 'Body' to 'This is body'
+6. Update 'Image URL' to 'https://d30y9cdsu7xlg0.cloudfront.net/png/205323-200.png'</t>
+  </si>
+  <si>
+    <t>Check for blank values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing should be displayed. </t>
+  </si>
+  <si>
+    <t>1. Erase the values in 'Header' and leave it blank
+2. Erase the values in 'Body' and leave it blank
+3. Hover on the Visual</t>
   </si>
 </sst>
 </file>
@@ -281,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -303,10 +354,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,6 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,16 +682,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956C572-3390-4C5B-816D-9D0DD3C60BEE}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="46.42578125" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
     <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" style="1" customWidth="1"/>
   </cols>
@@ -658,58 +710,121 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>12</v>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -721,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E27575F-1D23-4DE3-AE9F-04842A5F8AD7}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -733,13 +848,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -747,10 +862,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -758,10 +873,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -769,10 +884,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,10 +895,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -791,10 +906,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -802,10 +917,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -813,10 +928,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,10 +939,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,10 +950,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -846,10 +961,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -857,10 +972,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -868,10 +983,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -879,10 +994,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,10 +1005,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -901,10 +1016,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,35 +1027,35 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="9"/>
-    </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,30 +1063,30 @@
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="13"/>
     </row>
@@ -980,10 +1095,10 @@
         <v>19</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,10 +1106,10 @@
         <v>20</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>